<commit_message>
Update on Food Webs metadata
</commit_message>
<xml_diff>
--- a/MarineFoodWebs_Metadata.xlsx
+++ b/MarineFoodWebs_Metadata.xlsx
@@ -71,6 +71,34 @@
     <t>2</t>
   </si>
   <si>
+    <t>Baja California</t>
+  </si>
+  <si>
+    <t>121°54’30.7" W</t>
+  </si>
+  <si>
+    <t>36°47’52.3" N</t>
+  </si>
+  <si>
+    <t>1959-1961</t>
+  </si>
+  <si>
+    <t>Glynn PW. Community composition, structure, and interrelationships in the marine intertidal Endocladia muricata–Balanus glandula association in Monterey Bay, California. Beaufortia. 1965;12: 1–98.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://repository.naturalis.nl/pub/504945</t>
+    </r>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Baltic Sea</t>
   </si>
   <si>
@@ -99,7 +127,7 @@
     </r>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t>Barents Sea Arctic</t>
@@ -127,7 +155,7 @@
     </r>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t>Barents Sea Boreal</t>
@@ -139,7 +167,7 @@
     <t>73°06’28.6" N</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>Beach Peru</t>
@@ -157,7 +185,7 @@
     <t>NA</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Beagle Channel</t>
@@ -188,7 +216,7 @@
     </r>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Benguela</t>
@@ -213,7 +241,7 @@
     </r>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>Caribbean reef (l)</t>
@@ -238,7 +266,7 @@
     </r>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>Cayman Islands</t>
@@ -266,7 +294,7 @@
     </r>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>Celtic Sea</t>
@@ -294,7 +322,7 @@
     </r>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>Chilean rocky</t>
@@ -322,7 +350,7 @@
     </r>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>Cuba</t>
@@ -334,7 +362,7 @@
     <t>21°42’01.0" N</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>Florida</t>
@@ -359,7 +387,7 @@
     </r>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Gulf of Alaska</t>
@@ -387,7 +415,7 @@
     </r>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>Gulf of Cadiz</t>
@@ -412,7 +440,7 @@
     </r>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>Gulf of Lions</t>
@@ -440,7 +468,7 @@
     </r>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>Gulf of Tortugas</t>
@@ -468,7 +496,7 @@
     </r>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Jamaica</t>
@@ -480,7 +508,7 @@
     <t>17°45’40.3" N</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>La Guajira</t>
@@ -498,22 +526,40 @@
     <t>Criales-Hernández MI, B García C, Wolff M. Flujos de biomasa y estructura de un ecosistema de surgencia tropical en La Guajira, Caribe colombiano. Revista de biología tropical. 2006;54: 1257–82.</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Monterey Bay</t>
-  </si>
-  <si>
-    <t>121°54’30.7" W</t>
-  </si>
-  <si>
-    <t>36°47’52.3" N</t>
-  </si>
-  <si>
-    <t>1959-1961</t>
-  </si>
-  <si>
-    <t>Glynn PW. Community composition, structure, and interrelationships in the marine intertidal Endocladia muricata–Balanus glandula association in Monterey Bay, California. Beaufortia. 1965;12: 1–98.</t>
+    <t>21</t>
+  </si>
+  <si>
+    <t>NE US Shelf</t>
+  </si>
+  <si>
+    <t>68°16’18.9" W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43°49’36.8" N </t>
+  </si>
+  <si>
+    <t>1973-2001</t>
+  </si>
+  <si>
+    <t>Link J. Does food web theory work for marine ecosystems?. Marine ecology progress series. 2002;230: 1–9.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3354/meps230001</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Potter Cove</t>
+  </si>
+  <si>
+    <t>58°40’ W</t>
+  </si>
+  <si>
+    <t>62°14’ S</t>
+  </si>
+  <si>
+    <t>Marina TI, Salinas V, Cordone G, Campana G, Moreira E, Deregibus D, Torre L, Sahade R, Tatián M, Barrera Oro E, De Troch M, Doyle S, Quartino ML, Saravia LA, Momo FR. The Food Web of Potter Cove (Antarctica): complexity, structure and function. Estuarine, Coastal and Shelf Science.2018;200: 141–151.</t>
   </si>
   <si>
     <r>
@@ -522,32 +568,11 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>https://repository.naturalis.nl/pub/504945</t>
+      <t>https://doi.org/10.1016/j.ecss.2017.10.015</t>
     </r>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>NE US Shelf</t>
-  </si>
-  <si>
-    <t>68°16’18.9" W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43°49’36.8" N </t>
-  </si>
-  <si>
-    <t>1973-2001</t>
-  </si>
-  <si>
-    <t>Link J. Does food web theory work for marine ecosystems?. Marine ecology progress series. 2002;230: 1–9.</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.3354/meps230001</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>Sanak intertidal</t>
@@ -575,13 +600,13 @@
     </r>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>Sanak nearshore</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>Simon Bay</t>
@@ -609,7 +634,7 @@
     </r>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Southern Brazil</t>
@@ -637,7 +662,7 @@
     </r>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>SW Pacific Ocean</t>
@@ -665,7 +690,7 @@
     </r>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>Weddell Sea</t>
@@ -690,31 +715,6 @@
         <rFont val="Arial"/>
       </rPr>
       <t>https://doi.org/10.1016/B978-0-12-386475-8.00005-8</t>
-    </r>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Potter Cove</t>
-  </si>
-  <si>
-    <t>58°40’ W</t>
-  </si>
-  <si>
-    <t>62°14’ S</t>
-  </si>
-  <si>
-    <t>Marina TI, Salinas V, Cordone G, Campana G, Moreira E, Deregibus D, Torre L, Sahade R, Tatián M, Barrera Oro E, De Troch M, Doyle S, Quartino ML, Saravia LA, Momo FR. The Food Web of Potter Cove (Antarctica): complexity, structure and function. Estuarine, Coastal and Shelf Science.2018;200: 141–151.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>https://doi.org/10.1016/j.ecss.2017.10.015</t>
     </r>
   </si>
 </sst>
@@ -753,7 +753,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -763,6 +763,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -896,25 +902,25 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -937,6 +943,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2010,8 +2017,8 @@
     <col min="4" max="4" width="13.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.67188" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="62.9297" style="1" customWidth="1"/>
-    <col min="8" max="8" width="53.5938" style="1" customWidth="1"/>
+    <col min="7" max="7" width="63" style="1" customWidth="1"/>
+    <col min="8" max="8" width="53.6719" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2084,33 +2091,33 @@
         <v>20</v>
       </c>
       <c r="F3" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="H3" t="s" s="6">
         <v>22</v>
-      </c>
-      <c r="H3" t="s" s="6">
-        <v>23</v>
       </c>
     </row>
     <row r="4" ht="38.6" customHeight="1">
       <c r="A4" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="C4" t="s" s="8">
         <v>25</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="D4" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="D4" t="s" s="6">
+      <c r="E4" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E4" t="s" s="6">
+      <c r="F4" t="s" s="6">
         <v>28</v>
-      </c>
-      <c r="F4" t="s" s="6">
-        <v>21</v>
       </c>
       <c r="G4" t="s" s="6">
         <v>29</v>
@@ -2133,137 +2140,137 @@
         <v>34</v>
       </c>
       <c r="E5" t="s" s="6">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s" s="6">
         <v>28</v>
       </c>
-      <c r="F5" t="s" s="6">
-        <v>21</v>
-      </c>
       <c r="G5" t="s" s="6">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s" s="6">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="38.6" customHeight="1">
       <c r="A6" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s" s="6">
         <v>35</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="F6" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s" s="6">
         <v>36</v>
       </c>
-      <c r="C6" t="s" s="8">
+      <c r="H6" t="s" s="6">
         <v>37</v>
-      </c>
-      <c r="D6" t="s" s="6">
-        <v>38</v>
-      </c>
-      <c r="E6" s="9">
-        <v>1952</v>
-      </c>
-      <c r="F6" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s" s="6">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s" s="6">
-        <v>40</v>
       </c>
     </row>
     <row r="7" ht="38.6" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s" s="8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s" s="6">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s" s="6">
         <v>45</v>
       </c>
+      <c r="E7" s="9">
+        <v>1952</v>
+      </c>
       <c r="F7" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s" s="6">
         <v>46</v>
       </c>
-      <c r="G7" t="s" s="6">
+      <c r="H7" t="s" s="6">
         <v>47</v>
-      </c>
-      <c r="H7" t="s" s="6">
-        <v>48</v>
       </c>
     </row>
     <row r="8" ht="38.6" customHeight="1">
       <c r="A8" t="s" s="6">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s" s="7">
         <v>49</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="C8" t="s" s="8">
         <v>50</v>
       </c>
-      <c r="C8" t="s" s="8">
+      <c r="D8" t="s" s="6">
         <v>51</v>
       </c>
-      <c r="D8" t="s" s="6">
+      <c r="E8" t="s" s="6">
         <v>52</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s" s="6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" ht="38.6" customHeight="1">
+      <c r="A9" t="s" s="6">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>59</v>
+      </c>
+      <c r="E9" s="9">
         <v>1991</v>
       </c>
-      <c r="F8" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s" s="6">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s" s="6">
-        <v>54</v>
+      <c r="F9" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>61</v>
       </c>
     </row>
-    <row r="9" ht="26.6" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s" s="8">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>58</v>
-      </c>
-      <c r="E9" s="9">
+    <row r="10" ht="26.6" customHeight="1">
+      <c r="A10" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>65</v>
+      </c>
+      <c r="E10" s="9">
         <v>1967</v>
-      </c>
-      <c r="F9" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s" s="6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" ht="38.6" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>61</v>
-      </c>
-      <c r="B10" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="C10" t="s" s="8">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s" s="6">
-        <v>65</v>
       </c>
       <c r="F10" t="s" s="6">
         <v>13</v>
@@ -2301,7 +2308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" ht="40" customHeight="1">
+    <row r="12" ht="38.6" customHeight="1">
       <c r="A12" t="s" s="6">
         <v>75</v>
       </c>
@@ -2318,7 +2325,7 @@
         <v>79</v>
       </c>
       <c r="F12" t="s" s="6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s" s="6">
         <v>80</v>
@@ -2327,7 +2334,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" ht="38.6" customHeight="1">
+    <row r="13" ht="40" customHeight="1">
       <c r="A13" t="s" s="6">
         <v>82</v>
       </c>
@@ -2341,59 +2348,59 @@
         <v>85</v>
       </c>
       <c r="E13" t="s" s="6">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s" s="6">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s" s="6">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s" s="6">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" ht="38.6" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s" s="7">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s" s="8">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s" s="6">
-        <v>89</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1994</v>
+        <v>92</v>
+      </c>
+      <c r="E14" t="s" s="6">
+        <v>72</v>
       </c>
       <c r="F14" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G14" t="s" s="6">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s" s="6">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="15" ht="50.6" customHeight="1">
+    <row r="15" ht="38.6" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s" s="8">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>95</v>
-      </c>
-      <c r="E15" t="s" s="6">
         <v>96</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1994</v>
       </c>
       <c r="F15" t="s" s="6">
         <v>13</v>
@@ -2405,7 +2412,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" ht="38.6" customHeight="1">
+    <row r="16" ht="50.6" customHeight="1">
       <c r="A16" t="s" s="6">
         <v>99</v>
       </c>
@@ -2418,37 +2425,37 @@
       <c r="D16" t="s" s="6">
         <v>102</v>
       </c>
-      <c r="E16" s="9">
-        <v>2009</v>
+      <c r="E16" t="s" s="6">
+        <v>103</v>
       </c>
       <c r="F16" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G16" t="s" s="6">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H16" t="s" s="6">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="17" ht="50.6" customHeight="1">
+    <row r="17" ht="38.6" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s" s="8">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s" s="6">
-        <v>108</v>
-      </c>
-      <c r="E17" t="s" s="6">
         <v>109</v>
       </c>
+      <c r="E17" s="9">
+        <v>2009</v>
+      </c>
       <c r="F17" t="s" s="6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s" s="6">
         <v>110</v>
@@ -2457,7 +2464,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" ht="38.6" customHeight="1">
+    <row r="18" ht="50.6" customHeight="1">
       <c r="A18" t="s" s="6">
         <v>112</v>
       </c>
@@ -2474,7 +2481,7 @@
         <v>116</v>
       </c>
       <c r="F18" t="s" s="6">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s" s="6">
         <v>117</v>
@@ -2497,68 +2504,68 @@
         <v>122</v>
       </c>
       <c r="E19" t="s" s="6">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="F19" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G19" t="s" s="6">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="H19" t="s" s="6">
-        <v>67</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" ht="38.6" customHeight="1">
       <c r="A20" t="s" s="6">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s" s="8">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s" s="6">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s" s="6">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G20" t="s" s="6">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s" s="6">
-        <v>40</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" ht="38.6" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s" s="8">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s" s="6">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s" s="6">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F21" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G21" t="s" s="6">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H21" t="s" s="6">
-        <v>135</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" ht="26.6" customHeight="1">
@@ -2587,7 +2594,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" ht="38.6" customHeight="1">
+    <row r="23" ht="62.6" customHeight="1">
       <c r="A23" t="s" s="6">
         <v>143</v>
       </c>
@@ -2601,166 +2608,166 @@
         <v>146</v>
       </c>
       <c r="E23" t="s" s="6">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s" s="6">
         <v>147</v>
       </c>
-      <c r="F23" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s" s="6">
+      <c r="H23" t="s" s="6">
         <v>148</v>
-      </c>
-      <c r="H23" t="s" s="6">
-        <v>149</v>
       </c>
     </row>
     <row r="24" ht="38.6" customHeight="1">
       <c r="A24" t="s" s="6">
+        <v>149</v>
+      </c>
+      <c r="B24" t="s" s="7">
         <v>150</v>
       </c>
-      <c r="B24" t="s" s="7">
+      <c r="C24" t="s" s="8">
         <v>151</v>
       </c>
-      <c r="C24" t="s" s="8">
-        <v>145</v>
-      </c>
       <c r="D24" t="s" s="6">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s" s="6">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F24" t="s" s="6">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s" s="6">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="H24" t="s" s="6">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="25" ht="26.6" customHeight="1">
+    <row r="25" ht="38.6" customHeight="1">
       <c r="A25" t="s" s="6">
+        <v>156</v>
+      </c>
+      <c r="B25" t="s" s="7">
+        <v>157</v>
+      </c>
+      <c r="C25" t="s" s="8">
+        <v>151</v>
+      </c>
+      <c r="D25" t="s" s="6">
         <v>152</v>
       </c>
-      <c r="B25" t="s" s="7">
+      <c r="E25" t="s" s="6">
         <v>153</v>
       </c>
-      <c r="C25" t="s" s="8">
+      <c r="F25" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s" s="6">
         <v>154</v>
       </c>
-      <c r="D25" t="s" s="6">
+      <c r="H25" t="s" s="6">
         <v>155</v>
       </c>
-      <c r="E25" t="s" s="6">
-        <v>156</v>
-      </c>
-      <c r="F25" t="s" s="6">
-        <v>46</v>
-      </c>
-      <c r="G25" t="s" s="6">
-        <v>157</v>
-      </c>
-      <c r="H25" t="s" s="6">
+    </row>
+    <row r="26" ht="26.6" customHeight="1">
+      <c r="A26" t="s" s="6">
         <v>158</v>
       </c>
+      <c r="B26" t="s" s="7">
+        <v>159</v>
+      </c>
+      <c r="C26" t="s" s="8">
+        <v>160</v>
+      </c>
+      <c r="D26" t="s" s="6">
+        <v>161</v>
+      </c>
+      <c r="E26" t="s" s="6">
+        <v>162</v>
+      </c>
+      <c r="F26" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s" s="6">
+        <v>163</v>
+      </c>
+      <c r="H26" t="s" s="6">
+        <v>164</v>
+      </c>
     </row>
-    <row r="26" ht="40" customHeight="1">
-      <c r="A26" t="s" s="6">
-        <v>159</v>
-      </c>
-      <c r="B26" t="s" s="7">
-        <v>160</v>
-      </c>
-      <c r="C26" t="s" s="8">
-        <v>161</v>
-      </c>
-      <c r="D26" t="s" s="6">
-        <v>162</v>
-      </c>
-      <c r="E26" t="s" s="6">
-        <v>163</v>
-      </c>
-      <c r="F26" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s" s="6">
-        <v>164</v>
-      </c>
-      <c r="H26" t="s" s="6">
+    <row r="27" ht="40" customHeight="1">
+      <c r="A27" t="s" s="6">
         <v>165</v>
       </c>
-    </row>
-    <row r="27" ht="50.6" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="B27" t="s" s="7">
         <v>166</v>
       </c>
-      <c r="B27" t="s" s="7">
+      <c r="C27" t="s" s="8">
         <v>167</v>
       </c>
-      <c r="C27" t="s" s="8">
+      <c r="D27" t="s" s="6">
         <v>168</v>
       </c>
-      <c r="D27" t="s" s="6">
+      <c r="E27" t="s" s="6">
         <v>169</v>
-      </c>
-      <c r="E27" t="s" s="6">
-        <v>170</v>
       </c>
       <c r="F27" t="s" s="6">
         <v>13</v>
       </c>
       <c r="G27" t="s" s="6">
+        <v>170</v>
+      </c>
+      <c r="H27" t="s" s="6">
         <v>171</v>
-      </c>
-      <c r="H27" t="s" s="6">
-        <v>172</v>
       </c>
     </row>
     <row r="28" ht="50.6" customHeight="1">
       <c r="A28" t="s" s="6">
+        <v>172</v>
+      </c>
+      <c r="B28" t="s" s="7">
         <v>173</v>
       </c>
-      <c r="B28" t="s" s="7">
+      <c r="C28" t="s" s="8">
         <v>174</v>
       </c>
-      <c r="C28" t="s" s="8">
+      <c r="D28" t="s" s="6">
         <v>175</v>
       </c>
-      <c r="D28" t="s" s="6">
+      <c r="E28" t="s" s="6">
         <v>176</v>
       </c>
-      <c r="E28" t="s" s="6">
+      <c r="F28" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s" s="6">
         <v>177</v>
       </c>
-      <c r="F28" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="G28" t="s" s="6">
+      <c r="H28" t="s" s="6">
         <v>178</v>
       </c>
-      <c r="H28" t="s" s="6">
+    </row>
+    <row r="29" ht="50.6" customHeight="1">
+      <c r="A29" t="s" s="6">
         <v>179</v>
       </c>
-    </row>
-    <row r="29" ht="62.6" customHeight="1">
-      <c r="A29" t="s" s="6">
+      <c r="B29" t="s" s="7">
         <v>180</v>
       </c>
-      <c r="B29" t="s" s="7">
+      <c r="C29" t="s" s="8">
         <v>181</v>
       </c>
-      <c r="C29" t="s" s="8">
+      <c r="D29" t="s" s="6">
         <v>182</v>
       </c>
-      <c r="D29" t="s" s="6">
+      <c r="E29" t="s" s="6">
         <v>183</v>
       </c>
-      <c r="E29" t="s" s="6">
-        <v>40</v>
-      </c>
       <c r="F29" t="s" s="6">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G29" t="s" s="6">
         <v>184</v>
@@ -2772,30 +2779,30 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" location="" tooltip="" display="https://repositorio.ufrn.br/handle/123456789/30765"/>
-    <hyperlink ref="H3" r:id="rId2" location="" tooltip="" display="https://doi.org/10.1098/rspb.2015.2569"/>
-    <hyperlink ref="H4" r:id="rId3" location="" tooltip="" display="https://doi.org/10.1098/rspb.2015.1546"/>
+    <hyperlink ref="H3" r:id="rId2" location="" tooltip="" display="https://repository.naturalis.nl/pub/504945"/>
+    <hyperlink ref="H4" r:id="rId3" location="" tooltip="" display="https://doi.org/10.1098/rspb.2015.2569"/>
     <hyperlink ref="H5" r:id="rId4" location="" tooltip="" display="https://doi.org/10.1098/rspb.2015.1546"/>
-    <hyperlink ref="H7" r:id="rId5" location="" tooltip="" display="https://doi.org/10.1007/s00300-016-2007-x"/>
-    <hyperlink ref="H8" r:id="rId6" location="" tooltip="" display="https://doi.org/10.1046/j.1365-2656.1998.00224.x"/>
-    <hyperlink ref="H9" r:id="rId7" location="" tooltip="" display="https://www.researchgate.net/publication/227641407_Trophic_Interactions_in_Caribbean_Coral_Reefs"/>
-    <hyperlink ref="H10" r:id="rId8" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
-    <hyperlink ref="H11" r:id="rId9" location="" tooltip="" display="https://doi.org/10.1016/B978-0-12-385005-8.00006-X"/>
-    <hyperlink ref="H12" r:id="rId10" location="" tooltip="" display="https://doi.org/10.1890/13-1424.1"/>
-    <hyperlink ref="H13" r:id="rId11" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
-    <hyperlink ref="H14" r:id="rId12" location="" tooltip="" display="https://doi.org/10.1016/S0304-3800(99)00022-8"/>
-    <hyperlink ref="H15" r:id="rId13" location="" tooltip="" display="https://doi.org/10.1139/F08-104"/>
-    <hyperlink ref="H16" r:id="rId14" location="" tooltip="" display="https://doi.org/10.1016/j.ecolmodel.2013.05.019"/>
-    <hyperlink ref="H17" r:id="rId15" location="" tooltip="" display="https://doi.org/10.1016/j.jmarsys.2012.09.010"/>
-    <hyperlink ref="H18" r:id="rId16" location="" tooltip="" display="https://doi.org/10.1016/j.ecolmodel.2016.02.009"/>
-    <hyperlink ref="H19" r:id="rId17" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
-    <hyperlink ref="H21" r:id="rId18" location="" tooltip="" display="https://repository.naturalis.nl/pub/504945"/>
-    <hyperlink ref="H23" r:id="rId19" location="" tooltip="" display="https://doi.org/10.1038/srep21179"/>
+    <hyperlink ref="H6" r:id="rId5" location="" tooltip="" display="https://doi.org/10.1098/rspb.2015.1546"/>
+    <hyperlink ref="H8" r:id="rId6" location="" tooltip="" display="https://doi.org/10.1007/s00300-016-2007-x"/>
+    <hyperlink ref="H9" r:id="rId7" location="" tooltip="" display="https://doi.org/10.1046/j.1365-2656.1998.00224.x"/>
+    <hyperlink ref="H10" r:id="rId8" location="" tooltip="" display="https://www.researchgate.net/publication/227641407_Trophic_Interactions_in_Caribbean_Coral_Reefs"/>
+    <hyperlink ref="H11" r:id="rId9" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
+    <hyperlink ref="H12" r:id="rId10" location="" tooltip="" display="https://doi.org/10.1016/B978-0-12-385005-8.00006-X"/>
+    <hyperlink ref="H13" r:id="rId11" location="" tooltip="" display="https://doi.org/10.1890/13-1424.1"/>
+    <hyperlink ref="H14" r:id="rId12" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
+    <hyperlink ref="H15" r:id="rId13" location="" tooltip="" display="https://doi.org/10.1016/S0304-3800(99)00022-8"/>
+    <hyperlink ref="H16" r:id="rId14" location="" tooltip="" display="https://doi.org/10.1139/F08-104"/>
+    <hyperlink ref="H17" r:id="rId15" location="" tooltip="" display="https://doi.org/10.1016/j.ecolmodel.2013.05.019"/>
+    <hyperlink ref="H18" r:id="rId16" location="" tooltip="" display="https://doi.org/10.1016/j.jmarsys.2012.09.010"/>
+    <hyperlink ref="H19" r:id="rId17" location="" tooltip="" display="https://doi.org/10.1016/j.ecolmodel.2016.02.009"/>
+    <hyperlink ref="H20" r:id="rId18" location="" tooltip="" display="https://doi.org/10.7167/2013/857470"/>
+    <hyperlink ref="H23" r:id="rId19" location="" tooltip="" display="https://doi.org/10.1016/j.ecss.2017.10.015"/>
     <hyperlink ref="H24" r:id="rId20" location="" tooltip="" display="https://doi.org/10.1038/srep21179"/>
-    <hyperlink ref="H25" r:id="rId21" location="" tooltip="" display="https://doi.org/10.1016/j.csr.2010.10.010"/>
-    <hyperlink ref="H26" r:id="rId22" location="" tooltip="" display="https://doi.org/10.1111/maec.12407"/>
-    <hyperlink ref="H27" r:id="rId23" location="" tooltip="" display="https://doi.org/10.1016/j.pocean.2010.04.011"/>
-    <hyperlink ref="H28" r:id="rId24" location="" tooltip="" display="https://doi.org/10.1016/B978-0-12-386475-8.00005-8"/>
-    <hyperlink ref="H29" r:id="rId25" location="" tooltip="" display="https://doi.org/10.1016/j.ecss.2017.10.015"/>
+    <hyperlink ref="H25" r:id="rId21" location="" tooltip="" display="https://doi.org/10.1038/srep21179"/>
+    <hyperlink ref="H26" r:id="rId22" location="" tooltip="" display="https://doi.org/10.1016/j.csr.2010.10.010"/>
+    <hyperlink ref="H27" r:id="rId23" location="" tooltip="" display="https://doi.org/10.1111/maec.12407"/>
+    <hyperlink ref="H28" r:id="rId24" location="" tooltip="" display="https://doi.org/10.1016/j.pocean.2010.04.011"/>
+    <hyperlink ref="H29" r:id="rId25" location="" tooltip="" display="https://doi.org/10.1016/B978-0-12-386475-8.00005-8"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>